<commit_message>
first commit parent letter generation
</commit_message>
<xml_diff>
--- a/test data.xlsx
+++ b/test data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Apps\mentor_mentee_app_demo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A8435E-EBB6-4061-A7CD-DC2284D8BD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D6E63A-B41C-49EC-9103-D387B8F0636C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="324">
   <si>
     <t>Reg ID</t>
   </si>
@@ -814,6 +814,195 @@
   </si>
   <si>
     <t>HBoard1</t>
+  </si>
+  <si>
+    <t>mother's email</t>
+  </si>
+  <si>
+    <t>mother_email1</t>
+  </si>
+  <si>
+    <t>mother_email2</t>
+  </si>
+  <si>
+    <t>mother_email3</t>
+  </si>
+  <si>
+    <t>mother_email4</t>
+  </si>
+  <si>
+    <t>mother_email5</t>
+  </si>
+  <si>
+    <t>mother_email6</t>
+  </si>
+  <si>
+    <t>mother_email7</t>
+  </si>
+  <si>
+    <t>mother_email8</t>
+  </si>
+  <si>
+    <t>mother_email9</t>
+  </si>
+  <si>
+    <t>mother_email10</t>
+  </si>
+  <si>
+    <t>mother_email11</t>
+  </si>
+  <si>
+    <t>mother_email12</t>
+  </si>
+  <si>
+    <t>mother_email13</t>
+  </si>
+  <si>
+    <t>mother_email14</t>
+  </si>
+  <si>
+    <t>mother_email15</t>
+  </si>
+  <si>
+    <t>mother_email16</t>
+  </si>
+  <si>
+    <t>mother_email17</t>
+  </si>
+  <si>
+    <t>mother_email18</t>
+  </si>
+  <si>
+    <t>mother_email19</t>
+  </si>
+  <si>
+    <t>mother_email20</t>
+  </si>
+  <si>
+    <t>father's email</t>
+  </si>
+  <si>
+    <t>father_email1</t>
+  </si>
+  <si>
+    <t>father_email2</t>
+  </si>
+  <si>
+    <t>father_email3</t>
+  </si>
+  <si>
+    <t>father_email4</t>
+  </si>
+  <si>
+    <t>father_email5</t>
+  </si>
+  <si>
+    <t>father_email6</t>
+  </si>
+  <si>
+    <t>father_email7</t>
+  </si>
+  <si>
+    <t>father_email8</t>
+  </si>
+  <si>
+    <t>father_email9</t>
+  </si>
+  <si>
+    <t>father_email10</t>
+  </si>
+  <si>
+    <t>father_email11</t>
+  </si>
+  <si>
+    <t>father_email12</t>
+  </si>
+  <si>
+    <t>father_email13</t>
+  </si>
+  <si>
+    <t>father_email14</t>
+  </si>
+  <si>
+    <t>father_email15</t>
+  </si>
+  <si>
+    <t>father_email16</t>
+  </si>
+  <si>
+    <t>father_email17</t>
+  </si>
+  <si>
+    <t>father_email18</t>
+  </si>
+  <si>
+    <t>father_email19</t>
+  </si>
+  <si>
+    <t>father_email20</t>
+  </si>
+  <si>
+    <t>guardian's email</t>
+  </si>
+  <si>
+    <t>guardian_email 1</t>
+  </si>
+  <si>
+    <t>guardian_email 2</t>
+  </si>
+  <si>
+    <t>guardian_email 3</t>
+  </si>
+  <si>
+    <t>guardian_email 4</t>
+  </si>
+  <si>
+    <t>guardian_email 5</t>
+  </si>
+  <si>
+    <t>guardian_email 6</t>
+  </si>
+  <si>
+    <t>guardian_email 7</t>
+  </si>
+  <si>
+    <t>guardian_email 8</t>
+  </si>
+  <si>
+    <t>guardian_email 9</t>
+  </si>
+  <si>
+    <t>guardian_email 10</t>
+  </si>
+  <si>
+    <t>guardian_email 11</t>
+  </si>
+  <si>
+    <t>guardian_email 12</t>
+  </si>
+  <si>
+    <t>guardian_email 13</t>
+  </si>
+  <si>
+    <t>guardian_email 14</t>
+  </si>
+  <si>
+    <t>guardian_email 15</t>
+  </si>
+  <si>
+    <t>guardian_email 16</t>
+  </si>
+  <si>
+    <t>guardian_email 17</t>
+  </si>
+  <si>
+    <t>guardian_email 18</t>
+  </si>
+  <si>
+    <t>guardian_email 19</t>
+  </si>
+  <si>
+    <t>guardian_email 20</t>
   </si>
 </sst>
 </file>
@@ -1670,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU22"/>
+  <dimension ref="A1:AX22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AR4" sqref="AR4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1694,20 +1883,21 @@
     <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="18.77734375" customWidth="1"/>
-    <col min="29" max="29" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="44" width="14.88671875" customWidth="1"/>
-    <col min="45" max="45" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="23" width="18.77734375" customWidth="1"/>
+    <col min="32" max="32" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="14.88671875" customWidth="1"/>
+    <col min="48" max="48" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1757,100 +1947,109 @@
         <v>8</v>
       </c>
       <c r="Q1" t="s">
+        <v>261</v>
+      </c>
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
+        <v>282</v>
+      </c>
+      <c r="U1" t="s">
         <v>122</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>123</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
+        <v>303</v>
+      </c>
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>215</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>236</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>238</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>259</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>207</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>208</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>209</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>42</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>68293</v>
       </c>
@@ -1900,50 +2099,50 @@
         <v>43958923</v>
       </c>
       <c r="Q2" t="s">
+        <v>262</v>
+      </c>
+      <c r="R2" t="s">
         <v>14</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>234198515</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>283</v>
+      </c>
+      <c r="U2" t="s">
         <v>124</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>8546213246</v>
       </c>
-      <c r="U2">
+      <c r="W2" t="s">
+        <v>304</v>
+      </c>
+      <c r="X2">
         <v>89.34</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>216</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z2" t="s">
         <v>237</v>
       </c>
-      <c r="X2">
+      <c r="AA2">
         <v>85.34</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AB2" t="s">
         <v>239</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AC2" t="s">
         <v>260</v>
       </c>
-      <c r="AA2">
+      <c r="AD2">
         <v>103</v>
       </c>
-      <c r="AB2">
+      <c r="AE2">
         <v>250</v>
       </c>
-      <c r="AC2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>28</v>
-      </c>
       <c r="AF2" t="s">
         <v>28</v>
       </c>
@@ -1992,8 +2191,17 @@
       <c r="AU2" t="s">
         <v>28</v>
       </c>
+      <c r="AV2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>68294</v>
       </c>
@@ -2043,50 +2251,50 @@
         <v>23534622</v>
       </c>
       <c r="Q3" t="s">
+        <v>263</v>
+      </c>
+      <c r="R3" t="s">
         <v>18</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>543263276</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
+        <v>284</v>
+      </c>
+      <c r="U3" t="s">
         <v>125</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>8546213256</v>
       </c>
-      <c r="U3">
+      <c r="W3" t="s">
+        <v>305</v>
+      </c>
+      <c r="X3">
         <v>89.34</v>
       </c>
-      <c r="V3" t="s">
+      <c r="Y3" t="s">
         <v>217</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Z3" t="s">
         <v>237</v>
       </c>
-      <c r="X3">
+      <c r="AA3">
         <v>85.34</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AB3" t="s">
         <v>240</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AC3" t="s">
         <v>260</v>
       </c>
-      <c r="AA3">
+      <c r="AD3">
         <v>123</v>
       </c>
-      <c r="AB3">
+      <c r="AE3">
         <v>315</v>
       </c>
-      <c r="AC3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>28</v>
-      </c>
       <c r="AF3" t="s">
         <v>28</v>
       </c>
@@ -2135,8 +2343,17 @@
       <c r="AU3" t="s">
         <v>28</v>
       </c>
+      <c r="AV3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>68295</v>
       </c>
@@ -2186,50 +2403,50 @@
         <v>32592394</v>
       </c>
       <c r="Q4" t="s">
+        <v>264</v>
+      </c>
+      <c r="R4" t="s">
         <v>22</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>234093183</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
+        <v>285</v>
+      </c>
+      <c r="U4" t="s">
         <v>126</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>8546213266</v>
       </c>
-      <c r="U4">
+      <c r="W4" t="s">
+        <v>306</v>
+      </c>
+      <c r="X4">
         <v>89.34</v>
       </c>
-      <c r="V4" t="s">
+      <c r="Y4" t="s">
         <v>218</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Z4" t="s">
         <v>237</v>
       </c>
-      <c r="X4">
+      <c r="AA4">
         <v>85.34</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AB4" t="s">
         <v>241</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AC4" t="s">
         <v>260</v>
       </c>
-      <c r="AA4">
+      <c r="AD4">
         <v>141</v>
       </c>
-      <c r="AB4">
+      <c r="AE4">
         <v>361</v>
       </c>
-      <c r="AC4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>28</v>
-      </c>
       <c r="AF4" t="s">
         <v>28</v>
       </c>
@@ -2278,8 +2495,17 @@
       <c r="AU4" t="s">
         <v>28</v>
       </c>
+      <c r="AV4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>68296</v>
       </c>
@@ -2329,50 +2555,50 @@
         <v>32692394</v>
       </c>
       <c r="Q5" t="s">
+        <v>265</v>
+      </c>
+      <c r="R5" t="s">
         <v>96</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>576543563</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
+        <v>286</v>
+      </c>
+      <c r="U5" t="s">
         <v>127</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>8546213276</v>
       </c>
-      <c r="U5">
+      <c r="W5" t="s">
+        <v>307</v>
+      </c>
+      <c r="X5">
         <v>89.34</v>
       </c>
-      <c r="V5" t="s">
+      <c r="Y5" t="s">
         <v>219</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Z5" t="s">
         <v>237</v>
       </c>
-      <c r="X5">
+      <c r="AA5">
         <v>85.34</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="AB5" t="s">
         <v>242</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AC5" t="s">
         <v>260</v>
       </c>
-      <c r="AA5">
+      <c r="AD5">
         <v>134</v>
       </c>
-      <c r="AB5">
+      <c r="AE5">
         <v>234</v>
       </c>
-      <c r="AC5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>28</v>
-      </c>
       <c r="AF5" t="s">
         <v>28</v>
       </c>
@@ -2421,8 +2647,17 @@
       <c r="AU5" t="s">
         <v>28</v>
       </c>
+      <c r="AV5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>68297</v>
       </c>
@@ -2472,50 +2707,50 @@
         <v>32592393</v>
       </c>
       <c r="Q6" t="s">
+        <v>266</v>
+      </c>
+      <c r="R6" t="s">
         <v>97</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>457452456</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
+        <v>287</v>
+      </c>
+      <c r="U6" t="s">
         <v>128</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <v>8546213286</v>
       </c>
-      <c r="U6">
+      <c r="W6" t="s">
+        <v>308</v>
+      </c>
+      <c r="X6">
         <v>89.34</v>
       </c>
-      <c r="V6" t="s">
+      <c r="Y6" t="s">
         <v>220</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Z6" t="s">
         <v>237</v>
       </c>
-      <c r="X6">
+      <c r="AA6">
         <v>85.34</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AB6" t="s">
         <v>243</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AC6" t="s">
         <v>260</v>
       </c>
-      <c r="AA6">
+      <c r="AD6">
         <v>123</v>
       </c>
-      <c r="AB6">
+      <c r="AE6">
         <v>235</v>
       </c>
-      <c r="AC6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>28</v>
-      </c>
       <c r="AF6" t="s">
         <v>28</v>
       </c>
@@ -2564,8 +2799,17 @@
       <c r="AU6" t="s">
         <v>28</v>
       </c>
+      <c r="AV6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>68298</v>
       </c>
@@ -2615,50 +2859,50 @@
         <v>32492392</v>
       </c>
       <c r="Q7" t="s">
+        <v>267</v>
+      </c>
+      <c r="R7" t="s">
         <v>98</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>457455456</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
+        <v>288</v>
+      </c>
+      <c r="U7" t="s">
         <v>129</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <v>8546213296</v>
       </c>
-      <c r="U7">
+      <c r="W7" t="s">
+        <v>309</v>
+      </c>
+      <c r="X7">
         <v>89.34</v>
       </c>
-      <c r="V7" t="s">
+      <c r="Y7" t="s">
         <v>221</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Z7" t="s">
         <v>237</v>
       </c>
-      <c r="X7">
+      <c r="AA7">
         <v>85.34</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AB7" t="s">
         <v>244</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AC7" t="s">
         <v>260</v>
       </c>
-      <c r="AA7">
+      <c r="AD7">
         <v>132</v>
       </c>
-      <c r="AB7">
+      <c r="AE7">
         <v>238</v>
       </c>
-      <c r="AC7" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>28</v>
-      </c>
       <c r="AF7" t="s">
         <v>28</v>
       </c>
@@ -2707,8 +2951,17 @@
       <c r="AU7" t="s">
         <v>28</v>
       </c>
+      <c r="AV7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>68299</v>
       </c>
@@ -2758,50 +3011,50 @@
         <v>32392391</v>
       </c>
       <c r="Q8" t="s">
+        <v>268</v>
+      </c>
+      <c r="R8" t="s">
         <v>99</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>457458456</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
+        <v>289</v>
+      </c>
+      <c r="U8" t="s">
         <v>130</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <v>8546213306</v>
       </c>
-      <c r="U8">
+      <c r="W8" t="s">
+        <v>310</v>
+      </c>
+      <c r="X8">
         <v>89.34</v>
       </c>
-      <c r="V8" t="s">
+      <c r="Y8" t="s">
         <v>222</v>
       </c>
-      <c r="W8" t="s">
+      <c r="Z8" t="s">
         <v>237</v>
       </c>
-      <c r="X8">
+      <c r="AA8">
         <v>85.34</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AB8" t="s">
         <v>245</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AC8" t="s">
         <v>260</v>
       </c>
-      <c r="AA8">
+      <c r="AD8">
         <v>122</v>
       </c>
-      <c r="AB8">
+      <c r="AE8">
         <v>241</v>
       </c>
-      <c r="AC8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>28</v>
-      </c>
       <c r="AF8" t="s">
         <v>28</v>
       </c>
@@ -2850,8 +3103,17 @@
       <c r="AU8" t="s">
         <v>28</v>
       </c>
+      <c r="AV8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>68300</v>
       </c>
@@ -2901,50 +3163,50 @@
         <v>32292390</v>
       </c>
       <c r="Q9" t="s">
+        <v>269</v>
+      </c>
+      <c r="R9" t="s">
         <v>100</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>457461456</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
+        <v>290</v>
+      </c>
+      <c r="U9" t="s">
         <v>131</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>8546213316</v>
       </c>
-      <c r="U9">
+      <c r="W9" t="s">
+        <v>311</v>
+      </c>
+      <c r="X9">
         <v>89.34</v>
       </c>
-      <c r="V9" t="s">
+      <c r="Y9" t="s">
         <v>223</v>
       </c>
-      <c r="W9" t="s">
+      <c r="Z9" t="s">
         <v>237</v>
       </c>
-      <c r="X9">
+      <c r="AA9">
         <v>85.34</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="AB9" t="s">
         <v>246</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AC9" t="s">
         <v>260</v>
       </c>
-      <c r="AA9">
+      <c r="AD9">
         <v>112</v>
       </c>
-      <c r="AB9">
+      <c r="AE9">
         <v>244</v>
       </c>
-      <c r="AC9" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>28</v>
-      </c>
       <c r="AF9" t="s">
         <v>28</v>
       </c>
@@ -2993,8 +3255,17 @@
       <c r="AU9" t="s">
         <v>28</v>
       </c>
+      <c r="AV9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>68301</v>
       </c>
@@ -3044,50 +3315,50 @@
         <v>32192389</v>
       </c>
       <c r="Q10" t="s">
+        <v>270</v>
+      </c>
+      <c r="R10" t="s">
         <v>101</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>457464456</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
+        <v>291</v>
+      </c>
+      <c r="U10" t="s">
         <v>132</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>8546213326</v>
       </c>
-      <c r="U10">
+      <c r="W10" t="s">
+        <v>312</v>
+      </c>
+      <c r="X10">
         <v>89.34</v>
       </c>
-      <c r="V10" t="s">
+      <c r="Y10" t="s">
         <v>224</v>
       </c>
-      <c r="W10" t="s">
+      <c r="Z10" t="s">
         <v>237</v>
       </c>
-      <c r="X10">
+      <c r="AA10">
         <v>85.34</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="AB10" t="s">
         <v>247</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AC10" t="s">
         <v>260</v>
       </c>
-      <c r="AA10">
+      <c r="AD10">
         <v>123</v>
       </c>
-      <c r="AB10">
+      <c r="AE10">
         <v>247</v>
       </c>
-      <c r="AC10" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>28</v>
-      </c>
       <c r="AF10" t="s">
         <v>28</v>
       </c>
@@ -3136,8 +3407,17 @@
       <c r="AU10" t="s">
         <v>28</v>
       </c>
+      <c r="AV10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>68302</v>
       </c>
@@ -3187,50 +3467,50 @@
         <v>32092388</v>
       </c>
       <c r="Q11" t="s">
+        <v>271</v>
+      </c>
+      <c r="R11" t="s">
         <v>102</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>457467456</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
+        <v>292</v>
+      </c>
+      <c r="U11" t="s">
         <v>133</v>
       </c>
-      <c r="T11">
+      <c r="V11">
         <v>8546213336</v>
       </c>
-      <c r="U11">
+      <c r="W11" t="s">
+        <v>313</v>
+      </c>
+      <c r="X11">
         <v>89.34</v>
       </c>
-      <c r="V11" t="s">
+      <c r="Y11" t="s">
         <v>225</v>
       </c>
-      <c r="W11" t="s">
+      <c r="Z11" t="s">
         <v>237</v>
       </c>
-      <c r="X11">
+      <c r="AA11">
         <v>85.34</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="AB11" t="s">
         <v>248</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AC11" t="s">
         <v>260</v>
       </c>
-      <c r="AA11">
+      <c r="AD11">
         <v>141</v>
       </c>
-      <c r="AB11">
+      <c r="AE11">
         <v>250</v>
       </c>
-      <c r="AC11" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>28</v>
-      </c>
       <c r="AF11" t="s">
         <v>28</v>
       </c>
@@ -3279,8 +3559,17 @@
       <c r="AU11" t="s">
         <v>28</v>
       </c>
+      <c r="AV11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>68303</v>
       </c>
@@ -3330,50 +3619,50 @@
         <v>31992387</v>
       </c>
       <c r="Q12" t="s">
+        <v>272</v>
+      </c>
+      <c r="R12" t="s">
         <v>103</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>457470456</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
+        <v>293</v>
+      </c>
+      <c r="U12" t="s">
         <v>134</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>8546213346</v>
       </c>
-      <c r="U12">
+      <c r="W12" t="s">
+        <v>314</v>
+      </c>
+      <c r="X12">
         <v>89.34</v>
       </c>
-      <c r="V12" t="s">
+      <c r="Y12" t="s">
         <v>226</v>
       </c>
-      <c r="W12" t="s">
+      <c r="Z12" t="s">
         <v>237</v>
       </c>
-      <c r="X12">
+      <c r="AA12">
         <v>85.34</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="AB12" t="s">
         <v>249</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AC12" t="s">
         <v>260</v>
       </c>
-      <c r="AA12">
+      <c r="AD12">
         <v>145</v>
       </c>
-      <c r="AB12">
+      <c r="AE12">
         <v>253</v>
       </c>
-      <c r="AC12" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>28</v>
-      </c>
       <c r="AF12" t="s">
         <v>28</v>
       </c>
@@ -3422,8 +3711,17 @@
       <c r="AU12" t="s">
         <v>28</v>
       </c>
+      <c r="AV12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>68304</v>
       </c>
@@ -3473,50 +3771,50 @@
         <v>31892386</v>
       </c>
       <c r="Q13" t="s">
+        <v>273</v>
+      </c>
+      <c r="R13" t="s">
         <v>104</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>457473456</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
+        <v>294</v>
+      </c>
+      <c r="U13" t="s">
         <v>135</v>
       </c>
-      <c r="T13">
+      <c r="V13">
         <v>8546213356</v>
       </c>
-      <c r="U13">
+      <c r="W13" t="s">
+        <v>315</v>
+      </c>
+      <c r="X13">
         <v>89.34</v>
       </c>
-      <c r="V13" t="s">
+      <c r="Y13" t="s">
         <v>227</v>
       </c>
-      <c r="W13" t="s">
+      <c r="Z13" t="s">
         <v>237</v>
       </c>
-      <c r="X13">
+      <c r="AA13">
         <v>85.34</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="AB13" t="s">
         <v>250</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AC13" t="s">
         <v>260</v>
       </c>
-      <c r="AA13">
+      <c r="AD13">
         <v>149</v>
       </c>
-      <c r="AB13">
+      <c r="AE13">
         <v>256</v>
       </c>
-      <c r="AC13" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>28</v>
-      </c>
       <c r="AF13" t="s">
         <v>28</v>
       </c>
@@ -3565,8 +3863,17 @@
       <c r="AU13" t="s">
         <v>28</v>
       </c>
+      <c r="AV13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>68305</v>
       </c>
@@ -3616,50 +3923,50 @@
         <v>31792385</v>
       </c>
       <c r="Q14" t="s">
+        <v>274</v>
+      </c>
+      <c r="R14" t="s">
         <v>105</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>457476456</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
+        <v>295</v>
+      </c>
+      <c r="U14" t="s">
         <v>136</v>
       </c>
-      <c r="T14">
+      <c r="V14">
         <v>8546213366</v>
       </c>
-      <c r="U14">
+      <c r="W14" t="s">
+        <v>316</v>
+      </c>
+      <c r="X14">
         <v>89.34</v>
       </c>
-      <c r="V14" t="s">
+      <c r="Y14" t="s">
         <v>228</v>
       </c>
-      <c r="W14" t="s">
+      <c r="Z14" t="s">
         <v>237</v>
       </c>
-      <c r="X14">
+      <c r="AA14">
         <v>85.34</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="AB14" t="s">
         <v>251</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AC14" t="s">
         <v>260</v>
       </c>
-      <c r="AA14">
+      <c r="AD14">
         <v>153</v>
       </c>
-      <c r="AB14">
+      <c r="AE14">
         <v>259</v>
       </c>
-      <c r="AC14" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>28</v>
-      </c>
       <c r="AF14" t="s">
         <v>28</v>
       </c>
@@ -3708,8 +4015,17 @@
       <c r="AU14" t="s">
         <v>28</v>
       </c>
+      <c r="AV14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>68306</v>
       </c>
@@ -3759,50 +4075,50 @@
         <v>31692384</v>
       </c>
       <c r="Q15" t="s">
+        <v>275</v>
+      </c>
+      <c r="R15" t="s">
         <v>106</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>457479456</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
+        <v>296</v>
+      </c>
+      <c r="U15" t="s">
         <v>137</v>
       </c>
-      <c r="T15">
+      <c r="V15">
         <v>8546213376</v>
       </c>
-      <c r="U15">
+      <c r="W15" t="s">
+        <v>317</v>
+      </c>
+      <c r="X15">
         <v>89.34</v>
       </c>
-      <c r="V15" t="s">
+      <c r="Y15" t="s">
         <v>229</v>
       </c>
-      <c r="W15" t="s">
+      <c r="Z15" t="s">
         <v>237</v>
       </c>
-      <c r="X15">
+      <c r="AA15">
         <v>85.34</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="AB15" t="s">
         <v>252</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AC15" t="s">
         <v>260</v>
       </c>
-      <c r="AA15">
+      <c r="AD15">
         <v>157</v>
       </c>
-      <c r="AB15">
+      <c r="AE15">
         <v>262</v>
       </c>
-      <c r="AC15" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>28</v>
-      </c>
       <c r="AF15" t="s">
         <v>28</v>
       </c>
@@ -3851,8 +4167,17 @@
       <c r="AU15" t="s">
         <v>28</v>
       </c>
+      <c r="AV15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>68307</v>
       </c>
@@ -3902,50 +4227,50 @@
         <v>31592383</v>
       </c>
       <c r="Q16" t="s">
+        <v>276</v>
+      </c>
+      <c r="R16" t="s">
         <v>107</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>457482456</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
+        <v>297</v>
+      </c>
+      <c r="U16" t="s">
         <v>138</v>
       </c>
-      <c r="T16">
+      <c r="V16">
         <v>8546213386</v>
       </c>
-      <c r="U16">
+      <c r="W16" t="s">
+        <v>318</v>
+      </c>
+      <c r="X16">
         <v>89.34</v>
       </c>
-      <c r="V16" t="s">
+      <c r="Y16" t="s">
         <v>230</v>
       </c>
-      <c r="W16" t="s">
+      <c r="Z16" t="s">
         <v>237</v>
       </c>
-      <c r="X16">
+      <c r="AA16">
         <v>85.34</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="AB16" t="s">
         <v>253</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AC16" t="s">
         <v>260</v>
       </c>
-      <c r="AA16">
+      <c r="AD16">
         <v>161</v>
       </c>
-      <c r="AB16">
+      <c r="AE16">
         <v>265</v>
       </c>
-      <c r="AC16" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>28</v>
-      </c>
       <c r="AF16" t="s">
         <v>28</v>
       </c>
@@ -3994,8 +4319,17 @@
       <c r="AU16" t="s">
         <v>28</v>
       </c>
+      <c r="AV16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>68308</v>
       </c>
@@ -4045,50 +4379,50 @@
         <v>31492382</v>
       </c>
       <c r="Q17" t="s">
+        <v>277</v>
+      </c>
+      <c r="R17" t="s">
         <v>108</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>457485456</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
+        <v>298</v>
+      </c>
+      <c r="U17" t="s">
         <v>139</v>
       </c>
-      <c r="T17">
+      <c r="V17">
         <v>8546213396</v>
       </c>
-      <c r="U17">
+      <c r="W17" t="s">
+        <v>319</v>
+      </c>
+      <c r="X17">
         <v>89.34</v>
       </c>
-      <c r="V17" t="s">
+      <c r="Y17" t="s">
         <v>231</v>
       </c>
-      <c r="W17" t="s">
+      <c r="Z17" t="s">
         <v>237</v>
       </c>
-      <c r="X17">
+      <c r="AA17">
         <v>85.34</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="AB17" t="s">
         <v>254</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AC17" t="s">
         <v>260</v>
       </c>
-      <c r="AA17">
+      <c r="AD17">
         <v>165</v>
       </c>
-      <c r="AB17">
+      <c r="AE17">
         <v>268</v>
       </c>
-      <c r="AC17" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>28</v>
-      </c>
       <c r="AF17" t="s">
         <v>28</v>
       </c>
@@ -4137,8 +4471,17 @@
       <c r="AU17" t="s">
         <v>28</v>
       </c>
+      <c r="AV17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>68309</v>
       </c>
@@ -4188,50 +4531,50 @@
         <v>31392381</v>
       </c>
       <c r="Q18" t="s">
+        <v>278</v>
+      </c>
+      <c r="R18" t="s">
         <v>109</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>457488456</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
+        <v>299</v>
+      </c>
+      <c r="U18" t="s">
         <v>140</v>
       </c>
-      <c r="T18">
+      <c r="V18">
         <v>8546213406</v>
       </c>
-      <c r="U18">
+      <c r="W18" t="s">
+        <v>320</v>
+      </c>
+      <c r="X18">
         <v>89.34</v>
       </c>
-      <c r="V18" t="s">
+      <c r="Y18" t="s">
         <v>232</v>
       </c>
-      <c r="W18" t="s">
+      <c r="Z18" t="s">
         <v>237</v>
       </c>
-      <c r="X18">
+      <c r="AA18">
         <v>85.34</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="AB18" t="s">
         <v>255</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AC18" t="s">
         <v>260</v>
       </c>
-      <c r="AA18">
+      <c r="AD18">
         <v>169</v>
       </c>
-      <c r="AB18">
+      <c r="AE18">
         <v>271</v>
       </c>
-      <c r="AC18" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>28</v>
-      </c>
       <c r="AF18" t="s">
         <v>28</v>
       </c>
@@ -4280,8 +4623,17 @@
       <c r="AU18" t="s">
         <v>28</v>
       </c>
+      <c r="AV18" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>68310</v>
       </c>
@@ -4331,50 +4683,50 @@
         <v>31292380</v>
       </c>
       <c r="Q19" t="s">
+        <v>279</v>
+      </c>
+      <c r="R19" t="s">
         <v>110</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>457491456</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
+        <v>300</v>
+      </c>
+      <c r="U19" t="s">
         <v>141</v>
       </c>
-      <c r="T19">
+      <c r="V19">
         <v>8546213416</v>
       </c>
-      <c r="U19">
+      <c r="W19" t="s">
+        <v>321</v>
+      </c>
+      <c r="X19">
         <v>89.34</v>
       </c>
-      <c r="V19" t="s">
+      <c r="Y19" t="s">
         <v>233</v>
       </c>
-      <c r="W19" t="s">
+      <c r="Z19" t="s">
         <v>237</v>
       </c>
-      <c r="X19">
+      <c r="AA19">
         <v>85.34</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="AB19" t="s">
         <v>256</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AC19" t="s">
         <v>260</v>
       </c>
-      <c r="AA19">
+      <c r="AD19">
         <v>173</v>
       </c>
-      <c r="AB19">
+      <c r="AE19">
         <v>274</v>
       </c>
-      <c r="AC19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>28</v>
-      </c>
       <c r="AF19" t="s">
         <v>28</v>
       </c>
@@ -4423,8 +4775,17 @@
       <c r="AU19" t="s">
         <v>28</v>
       </c>
+      <c r="AV19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>68311</v>
       </c>
@@ -4474,50 +4835,50 @@
         <v>31192379</v>
       </c>
       <c r="Q20" t="s">
+        <v>280</v>
+      </c>
+      <c r="R20" t="s">
         <v>111</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>457494456</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
+        <v>301</v>
+      </c>
+      <c r="U20" t="s">
         <v>142</v>
       </c>
-      <c r="T20">
+      <c r="V20">
         <v>8546213426</v>
       </c>
-      <c r="U20">
+      <c r="W20" t="s">
+        <v>322</v>
+      </c>
+      <c r="X20">
         <v>89.34</v>
       </c>
-      <c r="V20" t="s">
+      <c r="Y20" t="s">
         <v>234</v>
       </c>
-      <c r="W20" t="s">
+      <c r="Z20" t="s">
         <v>237</v>
       </c>
-      <c r="X20">
+      <c r="AA20">
         <v>85.34</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="AB20" t="s">
         <v>257</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AC20" t="s">
         <v>260</v>
       </c>
-      <c r="AA20">
+      <c r="AD20">
         <v>177</v>
       </c>
-      <c r="AB20">
+      <c r="AE20">
         <v>277</v>
       </c>
-      <c r="AC20" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE20" t="s">
-        <v>28</v>
-      </c>
       <c r="AF20" t="s">
         <v>28</v>
       </c>
@@ -4566,8 +4927,17 @@
       <c r="AU20" t="s">
         <v>28</v>
       </c>
+      <c r="AV20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX20" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>68312</v>
       </c>
@@ -4617,50 +4987,50 @@
         <v>31092378</v>
       </c>
       <c r="Q21" t="s">
+        <v>281</v>
+      </c>
+      <c r="R21" t="s">
         <v>112</v>
       </c>
-      <c r="R21">
+      <c r="S21">
         <v>457497456</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
+        <v>302</v>
+      </c>
+      <c r="U21" t="s">
         <v>143</v>
       </c>
-      <c r="T21">
+      <c r="V21">
         <v>8546213436</v>
       </c>
-      <c r="U21">
+      <c r="W21" t="s">
+        <v>323</v>
+      </c>
+      <c r="X21">
         <v>89.34</v>
       </c>
-      <c r="V21" t="s">
+      <c r="Y21" t="s">
         <v>235</v>
       </c>
-      <c r="W21" t="s">
+      <c r="Z21" t="s">
         <v>237</v>
       </c>
-      <c r="X21">
+      <c r="AA21">
         <v>85.34</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="AB21" t="s">
         <v>258</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="AC21" t="s">
         <v>260</v>
       </c>
-      <c r="AA21">
+      <c r="AD21">
         <v>181</v>
       </c>
-      <c r="AB21">
+      <c r="AE21">
         <v>280</v>
       </c>
-      <c r="AC21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>28</v>
-      </c>
       <c r="AF21" t="s">
         <v>28</v>
       </c>
@@ -4709,8 +5079,17 @@
       <c r="AU21" t="s">
         <v>28</v>
       </c>
+      <c r="AV21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX21" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
       <c r="K22" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last basic feature added, todo now is to make student detail window and email functionality after testing said features
</commit_message>
<xml_diff>
--- a/test data.xlsx
+++ b/test data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Apps\mentor_mentee_app_demo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D6E63A-B41C-49EC-9103-D387B8F0636C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDA9E3D-5765-4E22-A56E-457ABAECBFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="326">
   <si>
     <t>Reg ID</t>
   </si>
@@ -1003,6 +1003,12 @@
   </si>
   <si>
     <t>guardian_email 20</t>
+  </si>
+  <si>
+    <t>Diploma Institue</t>
+  </si>
+  <si>
+    <t>Diploma Board</t>
   </si>
 </sst>
 </file>
@@ -1859,10 +1865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX22"/>
+  <dimension ref="A1:AZ22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+      <selection activeCell="AV23" sqref="AV23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1887,17 +1893,19 @@
     <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="23" width="18.77734375" customWidth="1"/>
     <col min="32" max="32" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="14.88671875" customWidth="1"/>
-    <col min="48" max="48" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="14.88671875" customWidth="1"/>
+    <col min="50" max="50" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1995,61 +2003,67 @@
         <v>27</v>
       </c>
       <c r="AG1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AI1" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>207</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>208</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>209</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>68293</v>
       </c>
@@ -2200,8 +2214,14 @@
       <c r="AX2" t="s">
         <v>28</v>
       </c>
+      <c r="AY2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>68294</v>
       </c>
@@ -2352,8 +2372,14 @@
       <c r="AX3" t="s">
         <v>28</v>
       </c>
+      <c r="AY3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>68295</v>
       </c>
@@ -2504,8 +2530,14 @@
       <c r="AX4" t="s">
         <v>28</v>
       </c>
+      <c r="AY4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>68296</v>
       </c>
@@ -2656,8 +2688,14 @@
       <c r="AX5" t="s">
         <v>28</v>
       </c>
+      <c r="AY5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>68297</v>
       </c>
@@ -2808,8 +2846,14 @@
       <c r="AX6" t="s">
         <v>28</v>
       </c>
+      <c r="AY6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>68298</v>
       </c>
@@ -2960,8 +3004,14 @@
       <c r="AX7" t="s">
         <v>28</v>
       </c>
+      <c r="AY7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>68299</v>
       </c>
@@ -3112,8 +3162,14 @@
       <c r="AX8" t="s">
         <v>28</v>
       </c>
+      <c r="AY8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>68300</v>
       </c>
@@ -3264,8 +3320,14 @@
       <c r="AX9" t="s">
         <v>28</v>
       </c>
+      <c r="AY9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>68301</v>
       </c>
@@ -3416,8 +3478,14 @@
       <c r="AX10" t="s">
         <v>28</v>
       </c>
+      <c r="AY10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>68302</v>
       </c>
@@ -3568,8 +3636,14 @@
       <c r="AX11" t="s">
         <v>28</v>
       </c>
+      <c r="AY11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>68303</v>
       </c>
@@ -3720,8 +3794,14 @@
       <c r="AX12" t="s">
         <v>28</v>
       </c>
+      <c r="AY12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>68304</v>
       </c>
@@ -3872,8 +3952,14 @@
       <c r="AX13" t="s">
         <v>28</v>
       </c>
+      <c r="AY13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>68305</v>
       </c>
@@ -4024,8 +4110,14 @@
       <c r="AX14" t="s">
         <v>28</v>
       </c>
+      <c r="AY14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>68306</v>
       </c>
@@ -4176,8 +4268,14 @@
       <c r="AX15" t="s">
         <v>28</v>
       </c>
+      <c r="AY15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ15" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>68307</v>
       </c>
@@ -4328,8 +4426,14 @@
       <c r="AX16" t="s">
         <v>28</v>
       </c>
+      <c r="AY16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ16" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>68308</v>
       </c>
@@ -4480,8 +4584,14 @@
       <c r="AX17" t="s">
         <v>28</v>
       </c>
+      <c r="AY17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>68309</v>
       </c>
@@ -4632,8 +4742,14 @@
       <c r="AX18" t="s">
         <v>28</v>
       </c>
+      <c r="AY18" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ18" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>68310</v>
       </c>
@@ -4784,8 +4900,14 @@
       <c r="AX19" t="s">
         <v>28</v>
       </c>
+      <c r="AY19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ19" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>68311</v>
       </c>
@@ -4936,8 +5058,14 @@
       <c r="AX20" t="s">
         <v>28</v>
       </c>
+      <c r="AY20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ20" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>68312</v>
       </c>
@@ -5088,8 +5216,14 @@
       <c r="AX21" t="s">
         <v>28</v>
       </c>
+      <c r="AY21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ21" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.3">
       <c r="K22" s="1"/>
     </row>
   </sheetData>

</xml_diff>